<commit_message>
refactored code/ setup travis
</commit_message>
<xml_diff>
--- a/sprint_planning/TeamDMVWReport.xlsx
+++ b/sprint_planning/TeamDMVWReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mruna\Desktop\GEDCOM_Project\sprint_planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EA14BE-B126-471E-8DDF-6F1EA26071C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2F60CE-EA21-45F8-935A-D43EEB8B0394}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="30" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="30" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown README" sheetId="13" r:id="rId1"/>
@@ -2449,7 +2449,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2730,7 +2730,7 @@
         <v>187</v>
       </c>
       <c r="E16" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -2747,7 +2747,7 @@
         <v>187</v>
       </c>
       <c r="E17" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -3063,7 +3063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -3554,8 +3554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3723,7 +3723,7 @@
         <v>187</v>
       </c>
       <c r="D8" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="E8">
         <v>40</v>
@@ -3743,7 +3743,7 @@
         <v>187</v>
       </c>
       <c r="D9" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="E9">
         <v>40</v>
@@ -3853,8 +3853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added US18 and US25
</commit_message>
<xml_diff>
--- a/sprint_planning/TeamDMVWReport.xlsx
+++ b/sprint_planning/TeamDMVWReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mruna\Desktop\GEDCOM_Project\sprint_planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086D9B9F-054B-46FA-A7BA-26EAE747D34E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299B81B7-B352-40CE-BBD6-077E196DD006}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="30" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown README" sheetId="13" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="263">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -836,6 +836,33 @@
   </si>
   <si>
     <t>Avoid unneccessary waste in code. Use class properties and methods already defined.</t>
+  </si>
+  <si>
+    <t>us25_unique_first_names_inFamilies</t>
+  </si>
+  <si>
+    <t>sprint3_tests.py</t>
+  </si>
+  <si>
+    <t>test_us25_unique_first_names_inFamilies</t>
+  </si>
+  <si>
+    <t>us18_siblings_should_not_marry</t>
+  </si>
+  <si>
+    <t>test_us18_siblings_should_not_marry</t>
+  </si>
+  <si>
+    <t>Marriage Before Divorce</t>
+  </si>
+  <si>
+    <t>Marriage Before Death</t>
+  </si>
+  <si>
+    <t>First Cousins should not marry</t>
+  </si>
+  <si>
+    <t>Reject Illegitimate Dates</t>
   </si>
 </sst>
 </file>
@@ -2190,7 +2217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -2511,8 +2538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A19" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2929,7 +2956,7 @@
         <v>187</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -2946,7 +2973,7 @@
         <v>187</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -3662,8 +3689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="K1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4144,18 +4171,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="L1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4183,8 +4215,26 @@
       <c r="I1" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>113</v>
       </c>
@@ -4204,7 +4254,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>114</v>
       </c>
@@ -4224,7 +4274,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>135</v>
       </c>
@@ -4244,7 +4294,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>150</v>
       </c>
@@ -4264,7 +4314,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>140</v>
       </c>
@@ -4284,7 +4334,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>132</v>
       </c>
@@ -4304,7 +4354,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>136</v>
       </c>
@@ -4315,7 +4365,7 @@
         <v>187</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="E8">
         <v>40</v>
@@ -4323,8 +4373,35 @@
       <c r="F8">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>60</v>
+      </c>
+      <c r="I8" t="s">
+        <v>233</v>
+      </c>
+      <c r="J8" t="s">
+        <v>234</v>
+      </c>
+      <c r="K8" t="s">
+        <v>254</v>
+      </c>
+      <c r="L8">
+        <v>585</v>
+      </c>
+      <c r="M8" t="s">
+        <v>255</v>
+      </c>
+      <c r="N8" t="s">
+        <v>256</v>
+      </c>
+      <c r="O8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>129</v>
       </c>
@@ -4335,13 +4412,40 @@
         <v>187</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="E9">
         <v>30</v>
       </c>
       <c r="F9">
         <v>60</v>
+      </c>
+      <c r="G9">
+        <v>12</v>
+      </c>
+      <c r="H9">
+        <v>30</v>
+      </c>
+      <c r="I9" t="s">
+        <v>233</v>
+      </c>
+      <c r="J9" t="s">
+        <v>234</v>
+      </c>
+      <c r="K9" t="s">
+        <v>257</v>
+      </c>
+      <c r="L9">
+        <v>604</v>
+      </c>
+      <c r="M9" t="s">
+        <v>255</v>
+      </c>
+      <c r="N9" t="s">
+        <v>258</v>
+      </c>
+      <c r="O9">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -4352,15 +4456,24 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4387,6 +4500,112 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" t="s">
+        <v>261</v>
+      </c>
+      <c r="C4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -4399,8 +4618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4673,7 +4892,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>135</v>
       </c>

</xml_diff>

<commit_message>
us29,us 10 both tested and test file
us 29 list decease
us 10 marry after 14
2 test case
and some change in the test gedcom file
</commit_message>
<xml_diff>
--- a/sprint_planning/TeamDMVWReport.xlsx
+++ b/sprint_planning/TeamDMVWReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mruna\Desktop\GEDCOM_Project\sprint_planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\54783\Desktop\GEDCOM\GEDCOM_Project\sprint_planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299B81B7-B352-40CE-BBD6-077E196DD006}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF035B4-8A07-472A-BD2C-8CE19EB2B824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown README" sheetId="13" r:id="rId1"/>
@@ -31,9 +31,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -44,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="265">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -863,6 +861,14 @@
   </si>
   <si>
     <t>Reject Illegitimate Dates</t>
+  </si>
+  <si>
+    <t>US21</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -870,10 +876,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="m/d"/>
+    <numFmt numFmtId="177" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -918,6 +924,12 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1016,20 +1028,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1037,7 +1049,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1053,75 +1065,75 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="65" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="64" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1139,7 +1151,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1276,7 +1288,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1305,10 +1317,10 @@
                   <c:v>09/17/2019</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10-1</c:v>
+                  <c:v>10/1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10-15</c:v>
+                  <c:v>10/15</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2221,47 +2233,47 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="7"/>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="7"/>
+    <col min="2" max="2" width="9.4609375" customWidth="1"/>
+    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3828125" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>159</v>
       </c>
@@ -2284,7 +2296,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>160</v>
       </c>
@@ -2300,7 +2312,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>161</v>
       </c>
@@ -2325,7 +2337,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>162</v>
       </c>
@@ -2350,7 +2362,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>163</v>
       </c>
@@ -2375,7 +2387,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>164</v>
       </c>
@@ -2401,6 +2413,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2415,16 +2428,16 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.453125" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
-    <col min="5" max="5" width="38.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.4609375" customWidth="1"/>
+    <col min="3" max="3" width="8.4609375" customWidth="1"/>
+    <col min="4" max="4" width="20.4609375" customWidth="1"/>
+    <col min="5" max="5" width="38.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2441,7 +2454,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>187</v>
       </c>
@@ -2458,7 +2471,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -2475,7 +2488,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>192</v>
       </c>
@@ -2492,7 +2505,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>201</v>
       </c>
@@ -2509,7 +2522,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2542,16 +2555,16 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.07421875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2568,7 +2581,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2585,7 +2598,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2602,7 +2615,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2619,7 +2632,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2636,7 +2649,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2653,7 +2666,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2670,7 +2683,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2687,7 +2700,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2704,7 +2717,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2721,7 +2734,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2738,7 +2751,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2755,7 +2768,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2772,7 +2785,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2789,7 +2802,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2806,7 +2819,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2823,7 +2836,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2840,7 +2853,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2857,7 +2870,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2874,7 +2887,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2891,7 +2904,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2908,7 +2921,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2925,7 +2938,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2942,7 +2955,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2959,7 +2972,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2976,7 +2989,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>4</v>
       </c>
@@ -2990,7 +3003,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>4</v>
       </c>
@@ -3004,7 +3017,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>4</v>
       </c>
@@ -3018,7 +3031,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>4</v>
       </c>
@@ -3032,7 +3045,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>4</v>
       </c>
@@ -3046,7 +3059,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>4</v>
       </c>
@@ -3060,7 +3073,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3074,7 +3087,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3103,17 +3116,17 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="2"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="2"/>
+    <col min="2" max="2" width="16.61328125" customWidth="1"/>
+    <col min="3" max="3" width="12.4609375" customWidth="1"/>
+    <col min="4" max="4" width="7.15234375" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3133,7 +3146,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>207</v>
       </c>
@@ -3144,7 +3157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>42277</v>
       </c>
@@ -3165,7 +3178,7 @@
         <v>273.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>42291</v>
       </c>
@@ -3198,30 +3211,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B21"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.08984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1796875" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.90625" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.61328125" customWidth="1"/>
+    <col min="2" max="2" width="24.4609375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.3828125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.61328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.3828125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.4609375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.07421875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.15234375" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.921875" style="17" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.08984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.07421875" style="17" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="34" style="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.15234375" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3268,7 +3281,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>127</v>
       </c>
@@ -3315,7 +3328,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>133</v>
       </c>
@@ -3362,7 +3375,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>125</v>
       </c>
@@ -3409,7 +3422,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>126</v>
       </c>
@@ -3456,7 +3469,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>141</v>
       </c>
@@ -3503,7 +3516,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>142</v>
       </c>
@@ -3550,7 +3563,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>144</v>
       </c>
@@ -3597,7 +3610,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>149</v>
       </c>
@@ -3644,36 +3657,36 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="21" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" ht="27" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>231</v>
       </c>
@@ -3689,21 +3702,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:O1"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.4609375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.4609375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.07421875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3750,9 +3763,9 @@
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>121</v>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>263</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>238</v>
@@ -3797,7 +3810,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>128</v>
       </c>
@@ -3844,7 +3857,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -3891,7 +3904,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3938,7 +3951,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>146</v>
       </c>
@@ -3985,7 +3998,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>147</v>
       </c>
@@ -4032,7 +4045,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>119</v>
       </c>
@@ -4079,7 +4092,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>120</v>
       </c>
@@ -4126,38 +4139,38 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B16" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="21" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="37.799999999999997" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" ht="40.5" x14ac:dyDescent="0.3">
       <c r="B20" s="21" t="s">
         <v>253</v>
       </c>
@@ -4173,21 +4186,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:O1"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.53515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.61328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4234,7 +4247,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>113</v>
       </c>
@@ -4254,7 +4267,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>114</v>
       </c>
@@ -4274,7 +4287,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>135</v>
       </c>
@@ -4294,7 +4307,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>150</v>
       </c>
@@ -4314,7 +4327,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>140</v>
       </c>
@@ -4334,9 +4347,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
-        <v>132</v>
+        <v>264</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>76</v>
@@ -4354,7 +4367,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>136</v>
       </c>
@@ -4401,7 +4414,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>129</v>
       </c>
@@ -4451,6 +4464,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4458,22 +4472,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.23046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.15234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.61328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.61328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4520,7 +4534,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -4531,7 +4545,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -4542,7 +4556,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>130</v>
       </c>
@@ -4553,7 +4567,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>153</v>
       </c>
@@ -4564,7 +4578,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -4575,7 +4589,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>115</v>
       </c>
@@ -4586,7 +4600,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>122</v>
       </c>
@@ -4597,7 +4611,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>151</v>
       </c>
@@ -4618,17 +4632,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>111</v>
       </c>
@@ -4639,7 +4653,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -4650,7 +4664,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -4661,7 +4675,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -4672,7 +4686,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -4683,7 +4697,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>116</v>
       </c>
@@ -4694,7 +4708,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -4705,7 +4719,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>118</v>
       </c>
@@ -4716,7 +4730,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>119</v>
       </c>
@@ -4727,7 +4741,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>120</v>
       </c>
@@ -4738,7 +4752,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>121</v>
       </c>
@@ -4749,7 +4763,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>122</v>
       </c>
@@ -4760,7 +4774,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>123</v>
       </c>
@@ -4771,7 +4785,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>124</v>
       </c>
@@ -4782,7 +4796,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>125</v>
       </c>
@@ -4793,7 +4807,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>126</v>
       </c>
@@ -4804,7 +4818,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>127</v>
       </c>
@@ -4815,7 +4829,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>128</v>
       </c>
@@ -4826,7 +4840,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>129</v>
       </c>
@@ -4837,7 +4851,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>130</v>
       </c>
@@ -4848,7 +4862,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>131</v>
       </c>
@@ -4859,7 +4873,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>132</v>
       </c>
@@ -4870,7 +4884,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>133</v>
       </c>
@@ -4881,7 +4895,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>134</v>
       </c>
@@ -4892,7 +4906,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>135</v>
       </c>
@@ -4903,7 +4917,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>136</v>
       </c>
@@ -4914,7 +4928,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>137</v>
       </c>
@@ -4925,7 +4939,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>138</v>
       </c>
@@ -4936,7 +4950,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>139</v>
       </c>
@@ -4947,7 +4961,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>140</v>
       </c>
@@ -4958,7 +4972,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>141</v>
       </c>
@@ -4969,7 +4983,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>142</v>
       </c>
@@ -4980,7 +4994,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>143</v>
       </c>
@@ -4991,7 +5005,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>144</v>
       </c>
@@ -5002,7 +5016,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>145</v>
       </c>
@@ -5013,7 +5027,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>146</v>
       </c>
@@ -5024,7 +5038,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>147</v>
       </c>
@@ -5035,7 +5049,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>148</v>
       </c>
@@ -5046,7 +5060,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>149</v>
       </c>
@@ -5057,7 +5071,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>150</v>
       </c>
@@ -5068,7 +5082,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>151</v>
       </c>
@@ -5079,7 +5093,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>152</v>
       </c>
@@ -5090,7 +5104,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>153</v>
       </c>
@@ -5102,6 +5116,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>

</xml_diff>